<commit_message>
fix score for cyfun
</commit_message>
<xml_diff>
--- a/tools/ccb/ccb-cff-2023-03-01.xlsx
+++ b/tools/ccb/ccb-cff-2023-03-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/ccb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B824AB6E-0787-8B45-B39C-FB71673B1340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC6BB1A-58AC-184B-8FEA-C488728ACD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -2947,14 +2947,6 @@
     <t>Formal processes, organisation oriented &amp; proactive</t>
   </si>
   <si>
-    <t>Formal processes, organisation oriented, controlled, proactive &amp;
-measured</t>
-  </si>
-  <si>
-    <t>Formal processes, organisation oriented, controlled, proactive,
-measured &amp; continual improvement focus</t>
-  </si>
-  <si>
     <t>scores</t>
   </si>
   <si>
@@ -2999,6 +2991,12 @@
   <si>
     <t>Centre For Cybersecurity Belgium - CyberFundamentals Framework
 https://ccb.belgium.be</t>
+  </si>
+  <si>
+    <t>Formal processes, organisation oriented, controlled, proactive &amp; measured</t>
+  </si>
+  <si>
+    <t>Formal processes, organisation oriented, controlled, proactive, measured &amp; continual improvement focus</t>
   </si>
 </sst>
 </file>
@@ -3383,7 +3381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B1651-6DC7-1E43-A5B6-8EF15B32842F}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="231" workbookViewId="0">
+    <sheetView zoomScale="231" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3439,7 +3437,7 @@
         <v>874</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -3514,10 +3512,10 @@
         <v>887</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="C15" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3525,10 +3523,10 @@
         <v>887</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C16" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
   </sheetData>
@@ -3564,7 +3562,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>864</v>
@@ -3623,7 +3621,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -3643,7 +3641,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -3663,7 +3661,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -3683,7 +3681,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -3714,7 +3712,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
@@ -3734,7 +3732,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
@@ -3754,7 +3752,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -3774,7 +3772,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D13" t="s">
         <v>35</v>
@@ -3794,7 +3792,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D14" t="s">
         <v>38</v>
@@ -3825,7 +3823,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D16" t="s">
         <v>43</v>
@@ -3845,7 +3843,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D17" t="s">
         <v>46</v>
@@ -3865,7 +3863,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D18" t="s">
         <v>49</v>
@@ -3896,7 +3894,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D20" t="s">
         <v>54</v>
@@ -3916,7 +3914,7 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D21" t="s">
         <v>57</v>
@@ -3947,7 +3945,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D23" t="s">
         <v>62</v>
@@ -3978,7 +3976,7 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D25" t="s">
         <v>67</v>
@@ -3998,7 +3996,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D26" t="s">
         <v>70</v>
@@ -4043,7 +4041,7 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D29" t="s">
         <v>78</v>
@@ -4063,7 +4061,7 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D30" t="s">
         <v>81</v>
@@ -4094,7 +4092,7 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D32" t="s">
         <v>890</v>
@@ -4125,7 +4123,7 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D34" t="s">
         <v>891</v>
@@ -4156,7 +4154,7 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D36" t="s">
         <v>892</v>
@@ -4187,7 +4185,7 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D38" t="s">
         <v>97</v>
@@ -4207,7 +4205,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D39" t="s">
         <v>100</v>
@@ -4227,7 +4225,7 @@
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D40" t="s">
         <v>103</v>
@@ -4272,7 +4270,7 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D43" t="s">
         <v>111</v>
@@ -4292,7 +4290,7 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D44" t="s">
         <v>114</v>
@@ -4323,7 +4321,7 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D46" t="s">
         <v>119</v>
@@ -4343,7 +4341,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D47" t="s">
         <v>122</v>
@@ -4374,7 +4372,7 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D49" t="s">
         <v>127</v>
@@ -4394,7 +4392,7 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D50" t="s">
         <v>130</v>
@@ -4439,7 +4437,7 @@
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D53" t="s">
         <v>138</v>
@@ -4459,7 +4457,7 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D54" t="s">
         <v>141</v>
@@ -4479,7 +4477,7 @@
         <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D55" t="s">
         <v>144</v>
@@ -4510,7 +4508,7 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D57" t="s">
         <v>149</v>
@@ -4530,7 +4528,7 @@
         <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D58" t="s">
         <v>152</v>
@@ -4561,7 +4559,7 @@
         <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D60" t="s">
         <v>156</v>
@@ -4581,7 +4579,7 @@
         <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D61" t="s">
         <v>159</v>
@@ -4601,7 +4599,7 @@
         <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D62" t="s">
         <v>162</v>
@@ -4632,7 +4630,7 @@
         <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D64" t="s">
         <v>166</v>
@@ -4677,7 +4675,7 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D67" t="s">
         <v>174</v>
@@ -4708,7 +4706,7 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D69" t="s">
         <v>179</v>
@@ -4739,7 +4737,7 @@
         <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D71" t="s">
         <v>184</v>
@@ -4784,7 +4782,7 @@
         <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D74" t="s">
         <v>191</v>
@@ -4815,7 +4813,7 @@
         <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D76" t="s">
         <v>195</v>
@@ -4835,7 +4833,7 @@
         <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D77" t="s">
         <v>198</v>
@@ -4866,7 +4864,7 @@
         <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D79" t="s">
         <v>203</v>
@@ -4886,7 +4884,7 @@
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D80" t="s">
         <v>206</v>
@@ -4906,7 +4904,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D81" t="s">
         <v>209</v>
@@ -4937,7 +4935,7 @@
         <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D83" t="s">
         <v>213</v>
@@ -4957,7 +4955,7 @@
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D84" t="s">
         <v>216</v>
@@ -4988,7 +4986,7 @@
         <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D86" t="s">
         <v>221</v>
@@ -5008,7 +5006,7 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D87" t="s">
         <v>223</v>
@@ -5064,13 +5062,13 @@
         <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D91" t="s">
         <v>232</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>233</v>
@@ -5084,7 +5082,7 @@
         <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D92" t="s">
         <v>234</v>
@@ -5104,7 +5102,7 @@
         <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D93" t="s">
         <v>237</v>
@@ -5124,7 +5122,7 @@
         <v>4</v>
       </c>
       <c r="C94" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D94" t="s">
         <v>240</v>
@@ -5144,7 +5142,7 @@
         <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D95" t="s">
         <v>243</v>
@@ -5175,7 +5173,7 @@
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D97" t="s">
         <v>248</v>
@@ -5195,7 +5193,7 @@
         <v>4</v>
       </c>
       <c r="C98" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D98" t="s">
         <v>251</v>
@@ -5215,7 +5213,7 @@
         <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D99" t="s">
         <v>254</v>
@@ -5235,7 +5233,7 @@
         <v>4</v>
       </c>
       <c r="C100" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D100" t="s">
         <v>257</v>
@@ -5266,7 +5264,7 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D102" t="s">
         <v>262</v>
@@ -5286,7 +5284,7 @@
         <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D103" t="s">
         <v>265</v>
@@ -5306,7 +5304,7 @@
         <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D104" t="s">
         <v>268</v>
@@ -5326,7 +5324,7 @@
         <v>4</v>
       </c>
       <c r="C105" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D105" t="s">
         <v>271</v>
@@ -5346,7 +5344,7 @@
         <v>4</v>
       </c>
       <c r="C106" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D106" t="s">
         <v>274</v>
@@ -5377,7 +5375,7 @@
         <v>4</v>
       </c>
       <c r="C108" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D108" t="s">
         <v>279</v>
@@ -5397,7 +5395,7 @@
         <v>4</v>
       </c>
       <c r="C109" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D109" t="s">
         <v>282</v>
@@ -5417,13 +5415,13 @@
         <v>4</v>
       </c>
       <c r="C110" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D110" t="s">
         <v>285</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="G110" s="4" t="s">
         <v>286</v>
@@ -5437,13 +5435,13 @@
         <v>4</v>
       </c>
       <c r="C111" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D111" t="s">
         <v>287</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="G111" s="4" t="s">
         <v>288</v>
@@ -5457,7 +5455,7 @@
         <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D112" t="s">
         <v>289</v>
@@ -5477,7 +5475,7 @@
         <v>4</v>
       </c>
       <c r="C113" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D113" t="s">
         <v>292</v>
@@ -5497,7 +5495,7 @@
         <v>4</v>
       </c>
       <c r="C114" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D114" t="s">
         <v>295</v>
@@ -5517,7 +5515,7 @@
         <v>4</v>
       </c>
       <c r="C115" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D115" t="s">
         <v>297</v>
@@ -5537,7 +5535,7 @@
         <v>4</v>
       </c>
       <c r="C116" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D116" t="s">
         <v>300</v>
@@ -5568,7 +5566,7 @@
         <v>4</v>
       </c>
       <c r="C118" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D118" t="s">
         <v>304</v>
@@ -5588,7 +5586,7 @@
         <v>4</v>
       </c>
       <c r="C119" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D119" t="s">
         <v>307</v>
@@ -5608,7 +5606,7 @@
         <v>4</v>
       </c>
       <c r="C120" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D120" t="s">
         <v>310</v>
@@ -5628,7 +5626,7 @@
         <v>4</v>
       </c>
       <c r="C121" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D121" t="s">
         <v>313</v>
@@ -5648,7 +5646,7 @@
         <v>4</v>
       </c>
       <c r="C122" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D122" t="s">
         <v>316</v>
@@ -5668,7 +5666,7 @@
         <v>4</v>
       </c>
       <c r="C123" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D123" t="s">
         <v>318</v>
@@ -5699,7 +5697,7 @@
         <v>4</v>
       </c>
       <c r="C125" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D125" t="s">
         <v>322</v>
@@ -5719,7 +5717,7 @@
         <v>4</v>
       </c>
       <c r="C126" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D126" t="s">
         <v>324</v>
@@ -5750,7 +5748,7 @@
         <v>4</v>
       </c>
       <c r="C128" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D128" t="s">
         <v>328</v>
@@ -5795,7 +5793,7 @@
         <v>4</v>
       </c>
       <c r="C131" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D131" t="s">
         <v>336</v>
@@ -5815,7 +5813,7 @@
         <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D132" t="s">
         <v>339</v>
@@ -5835,7 +5833,7 @@
         <v>4</v>
       </c>
       <c r="C133" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D133" t="s">
         <v>342</v>
@@ -5866,7 +5864,7 @@
         <v>4</v>
       </c>
       <c r="C135" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D135" t="s">
         <v>346</v>
@@ -5897,7 +5895,7 @@
         <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D137" t="s">
         <v>350</v>
@@ -5917,7 +5915,7 @@
         <v>4</v>
       </c>
       <c r="C138" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D138" t="s">
         <v>353</v>
@@ -5937,7 +5935,7 @@
         <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D139" t="s">
         <v>356</v>
@@ -5957,7 +5955,7 @@
         <v>4</v>
       </c>
       <c r="C140" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D140" t="s">
         <v>359</v>
@@ -5988,7 +5986,7 @@
         <v>4</v>
       </c>
       <c r="C142" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D142" t="s">
         <v>363</v>
@@ -6019,7 +6017,7 @@
         <v>4</v>
       </c>
       <c r="C144" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D144" t="s">
         <v>368</v>
@@ -6064,7 +6062,7 @@
         <v>4</v>
       </c>
       <c r="C147" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D147" t="s">
         <v>375</v>
@@ -6095,7 +6093,7 @@
         <v>4</v>
       </c>
       <c r="C149" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D149" t="s">
         <v>380</v>
@@ -6126,7 +6124,7 @@
         <v>4</v>
       </c>
       <c r="C151" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D151" t="s">
         <v>385</v>
@@ -6146,7 +6144,7 @@
         <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D152" t="s">
         <v>388</v>
@@ -6166,7 +6164,7 @@
         <v>4</v>
       </c>
       <c r="C153" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D153" t="s">
         <v>391</v>
@@ -6186,7 +6184,7 @@
         <v>4</v>
       </c>
       <c r="C154" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D154" t="s">
         <v>394</v>
@@ -6217,7 +6215,7 @@
         <v>4</v>
       </c>
       <c r="C156" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D156" t="s">
         <v>399</v>
@@ -6237,7 +6235,7 @@
         <v>4</v>
       </c>
       <c r="C157" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D157" t="s">
         <v>893</v>
@@ -6257,7 +6255,7 @@
         <v>4</v>
       </c>
       <c r="C158" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D158" t="s">
         <v>403</v>
@@ -6288,7 +6286,7 @@
         <v>4</v>
       </c>
       <c r="C160" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D160" t="s">
         <v>407</v>
@@ -6319,7 +6317,7 @@
         <v>4</v>
       </c>
       <c r="C162" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D162" t="s">
         <v>412</v>
@@ -6339,7 +6337,7 @@
         <v>4</v>
       </c>
       <c r="C163" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D163" t="s">
         <v>415</v>
@@ -6359,7 +6357,7 @@
         <v>4</v>
       </c>
       <c r="C164" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D164" t="s">
         <v>417</v>
@@ -6390,7 +6388,7 @@
         <v>4</v>
       </c>
       <c r="C166" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D166" t="s">
         <v>421</v>
@@ -6421,7 +6419,7 @@
         <v>4</v>
       </c>
       <c r="C168" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D168" t="s">
         <v>426</v>
@@ -6441,7 +6439,7 @@
         <v>4</v>
       </c>
       <c r="C169" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D169" t="s">
         <v>428</v>
@@ -6464,7 +6462,7 @@
         <v>431</v>
       </c>
       <c r="F170" s="4" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -6486,7 +6484,7 @@
         <v>4</v>
       </c>
       <c r="C172" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D172" t="s">
         <v>434</v>
@@ -6506,7 +6504,7 @@
         <v>4</v>
       </c>
       <c r="C173" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D173" t="s">
         <v>437</v>
@@ -6537,7 +6535,7 @@
         <v>4</v>
       </c>
       <c r="C175" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D175" t="s">
         <v>442</v>
@@ -6557,7 +6555,7 @@
         <v>4</v>
       </c>
       <c r="C176" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D176" t="s">
         <v>445</v>
@@ -6588,7 +6586,7 @@
         <v>4</v>
       </c>
       <c r="C178" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D178" t="s">
         <v>450</v>
@@ -6608,7 +6606,7 @@
         <v>4</v>
       </c>
       <c r="C179" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D179" t="s">
         <v>452</v>
@@ -6639,7 +6637,7 @@
         <v>4</v>
       </c>
       <c r="C181" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D181" t="s">
         <v>456</v>
@@ -6659,7 +6657,7 @@
         <v>4</v>
       </c>
       <c r="C182" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D182" t="s">
         <v>459</v>
@@ -6679,7 +6677,7 @@
         <v>4</v>
       </c>
       <c r="C183" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D183" t="s">
         <v>462</v>
@@ -6699,7 +6697,7 @@
         <v>4</v>
       </c>
       <c r="C184" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D184" t="s">
         <v>465</v>
@@ -6719,7 +6717,7 @@
         <v>4</v>
       </c>
       <c r="C185" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D185" t="s">
         <v>468</v>
@@ -6750,7 +6748,7 @@
         <v>4</v>
       </c>
       <c r="C187" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D187" t="s">
         <v>473</v>
@@ -6770,7 +6768,7 @@
         <v>4</v>
       </c>
       <c r="C188" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D188" t="s">
         <v>476</v>
@@ -6801,7 +6799,7 @@
         <v>4</v>
       </c>
       <c r="C190" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D190" t="s">
         <v>480</v>
@@ -6821,7 +6819,7 @@
         <v>4</v>
       </c>
       <c r="C191" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D191" t="s">
         <v>483</v>
@@ -6852,7 +6850,7 @@
         <v>4</v>
       </c>
       <c r="C193" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D193" t="s">
         <v>488</v>
@@ -6872,7 +6870,7 @@
         <v>4</v>
       </c>
       <c r="C194" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D194" t="s">
         <v>490</v>
@@ -6892,7 +6890,7 @@
         <v>4</v>
       </c>
       <c r="C195" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D195" t="s">
         <v>493</v>
@@ -6923,7 +6921,7 @@
         <v>4</v>
       </c>
       <c r="C197" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D197" t="s">
         <v>497</v>
@@ -6943,7 +6941,7 @@
         <v>4</v>
       </c>
       <c r="C198" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D198" t="s">
         <v>499</v>
@@ -6963,7 +6961,7 @@
         <v>4</v>
       </c>
       <c r="C199" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D199" t="s">
         <v>501</v>
@@ -6994,7 +6992,7 @@
         <v>4</v>
       </c>
       <c r="C201" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D201" t="s">
         <v>505</v>
@@ -7014,7 +7012,7 @@
         <v>4</v>
       </c>
       <c r="C202" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D202" t="s">
         <v>508</v>
@@ -7045,7 +7043,7 @@
         <v>4</v>
       </c>
       <c r="C204" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D204" t="s">
         <v>513</v>
@@ -7065,7 +7063,7 @@
         <v>4</v>
       </c>
       <c r="C205" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D205" t="s">
         <v>516</v>
@@ -7096,7 +7094,7 @@
         <v>4</v>
       </c>
       <c r="C207" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D207" t="s">
         <v>521</v>
@@ -7141,7 +7139,7 @@
         <v>4</v>
       </c>
       <c r="C210" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D210" t="s">
         <v>529</v>
@@ -7161,7 +7159,7 @@
         <v>4</v>
       </c>
       <c r="C211" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D211" t="s">
         <v>532</v>
@@ -7181,7 +7179,7 @@
         <v>4</v>
       </c>
       <c r="C212" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D212" t="s">
         <v>535</v>
@@ -7201,7 +7199,7 @@
         <v>4</v>
       </c>
       <c r="C213" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D213" t="s">
         <v>538</v>
@@ -7221,7 +7219,7 @@
         <v>4</v>
       </c>
       <c r="C214" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D214" t="s">
         <v>541</v>
@@ -7241,7 +7239,7 @@
         <v>4</v>
       </c>
       <c r="C215" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D215" t="s">
         <v>544</v>
@@ -7261,7 +7259,7 @@
         <v>4</v>
       </c>
       <c r="C216" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D216" t="s">
         <v>546</v>
@@ -7292,7 +7290,7 @@
         <v>4</v>
       </c>
       <c r="C218" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D218" t="s">
         <v>550</v>
@@ -7312,7 +7310,7 @@
         <v>4</v>
       </c>
       <c r="C219" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D219" t="s">
         <v>552</v>
@@ -7332,7 +7330,7 @@
         <v>4</v>
       </c>
       <c r="C220" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D220" t="s">
         <v>554</v>
@@ -7377,7 +7375,7 @@
         <v>4</v>
       </c>
       <c r="C223" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D223" t="s">
         <v>561</v>
@@ -7397,7 +7395,7 @@
         <v>4</v>
       </c>
       <c r="C224" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D224" t="s">
         <v>564</v>
@@ -7417,7 +7415,7 @@
         <v>4</v>
       </c>
       <c r="C225" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D225" t="s">
         <v>567</v>
@@ -7437,7 +7435,7 @@
         <v>4</v>
       </c>
       <c r="C226" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D226" t="s">
         <v>570</v>
@@ -7468,7 +7466,7 @@
         <v>4</v>
       </c>
       <c r="C228" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D228" t="s">
         <v>574</v>
@@ -7488,7 +7486,7 @@
         <v>4</v>
       </c>
       <c r="C229" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D229" t="s">
         <v>576</v>
@@ -7508,7 +7506,7 @@
         <v>4</v>
       </c>
       <c r="C230" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D230" t="s">
         <v>578</v>
@@ -7539,7 +7537,7 @@
         <v>4</v>
       </c>
       <c r="C232" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D232" t="s">
         <v>583</v>
@@ -7559,7 +7557,7 @@
         <v>4</v>
       </c>
       <c r="C233" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D233" t="s">
         <v>586</v>
@@ -7579,7 +7577,7 @@
         <v>4</v>
       </c>
       <c r="C234" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D234" t="s">
         <v>588</v>
@@ -7610,7 +7608,7 @@
         <v>4</v>
       </c>
       <c r="C236" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D236" t="s">
         <v>592</v>
@@ -7630,7 +7628,7 @@
         <v>4</v>
       </c>
       <c r="C237" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D237" t="s">
         <v>595</v>
@@ -7650,7 +7648,7 @@
         <v>4</v>
       </c>
       <c r="C238" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D238" t="s">
         <v>598</v>
@@ -7706,7 +7704,7 @@
         <v>4</v>
       </c>
       <c r="C242" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D242" t="s">
         <v>607</v>
@@ -7737,7 +7735,7 @@
         <v>4</v>
       </c>
       <c r="C244" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D244" t="s">
         <v>612</v>
@@ -7757,7 +7755,7 @@
         <v>4</v>
       </c>
       <c r="C245" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D245" t="s">
         <v>614</v>
@@ -7788,7 +7786,7 @@
         <v>4</v>
       </c>
       <c r="C247" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D247" t="s">
         <v>619</v>
@@ -7808,7 +7806,7 @@
         <v>4</v>
       </c>
       <c r="C248" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D248" t="s">
         <v>622</v>
@@ -7828,7 +7826,7 @@
         <v>4</v>
       </c>
       <c r="C249" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D249" t="s">
         <v>624</v>
@@ -7859,7 +7857,7 @@
         <v>4</v>
       </c>
       <c r="C251" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D251" t="s">
         <v>628</v>
@@ -7890,7 +7888,7 @@
         <v>4</v>
       </c>
       <c r="C253" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D253" t="s">
         <v>632</v>
@@ -7910,7 +7908,7 @@
         <v>4</v>
       </c>
       <c r="C254" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D254" t="s">
         <v>634</v>
@@ -7955,7 +7953,7 @@
         <v>4</v>
       </c>
       <c r="C257" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D257" t="s">
         <v>641</v>
@@ -7975,7 +7973,7 @@
         <v>4</v>
       </c>
       <c r="C258" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D258" t="s">
         <v>644</v>
@@ -7995,7 +7993,7 @@
         <v>4</v>
       </c>
       <c r="C259" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D259" t="s">
         <v>647</v>
@@ -8026,7 +8024,7 @@
         <v>4</v>
       </c>
       <c r="C261" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D261" t="s">
         <v>652</v>
@@ -8046,7 +8044,7 @@
         <v>4</v>
       </c>
       <c r="C262" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D262" t="s">
         <v>654</v>
@@ -8077,7 +8075,7 @@
         <v>4</v>
       </c>
       <c r="C264" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D264" t="s">
         <v>659</v>
@@ -8097,7 +8095,7 @@
         <v>4</v>
       </c>
       <c r="C265" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D265" t="s">
         <v>662</v>
@@ -8117,7 +8115,7 @@
         <v>4</v>
       </c>
       <c r="C266" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D266" t="s">
         <v>665</v>
@@ -8148,7 +8146,7 @@
         <v>4</v>
       </c>
       <c r="C268" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D268" t="s">
         <v>670</v>
@@ -8168,7 +8166,7 @@
         <v>4</v>
       </c>
       <c r="C269" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D269" t="s">
         <v>673</v>
@@ -8199,7 +8197,7 @@
         <v>4</v>
       </c>
       <c r="C271" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D271" t="s">
         <v>677</v>
@@ -8230,7 +8228,7 @@
         <v>4</v>
       </c>
       <c r="C273" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D273" t="s">
         <v>682</v>
@@ -8250,7 +8248,7 @@
         <v>4</v>
       </c>
       <c r="C274" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D274" t="s">
         <v>685</v>
@@ -8281,7 +8279,7 @@
         <v>4</v>
       </c>
       <c r="C276" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D276" t="s">
         <v>689</v>
@@ -8301,7 +8299,7 @@
         <v>4</v>
       </c>
       <c r="C277" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D277" t="s">
         <v>692</v>
@@ -8332,7 +8330,7 @@
         <v>4</v>
       </c>
       <c r="C279" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D279" t="s">
         <v>696</v>
@@ -8352,7 +8350,7 @@
         <v>4</v>
       </c>
       <c r="C280" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D280" t="s">
         <v>699</v>
@@ -8397,7 +8395,7 @@
         <v>4</v>
       </c>
       <c r="C283" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D283" t="s">
         <v>706</v>
@@ -8428,7 +8426,7 @@
         <v>4</v>
       </c>
       <c r="C285" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D285" t="s">
         <v>710</v>
@@ -8459,7 +8457,7 @@
         <v>4</v>
       </c>
       <c r="C287" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D287" t="s">
         <v>715</v>
@@ -8490,7 +8488,7 @@
         <v>4</v>
       </c>
       <c r="C289" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D289" t="s">
         <v>720</v>
@@ -8510,7 +8508,7 @@
         <v>4</v>
       </c>
       <c r="C290" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D290" t="s">
         <v>723</v>
@@ -8566,7 +8564,7 @@
         <v>4</v>
       </c>
       <c r="C294" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D294" t="s">
         <v>733</v>
@@ -8611,7 +8609,7 @@
         <v>4</v>
       </c>
       <c r="C297" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D297" t="s">
         <v>741</v>
@@ -8642,7 +8640,7 @@
         <v>4</v>
       </c>
       <c r="C299" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D299" t="s">
         <v>746</v>
@@ -8662,7 +8660,7 @@
         <v>4</v>
       </c>
       <c r="C300" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D300" t="s">
         <v>749</v>
@@ -8693,7 +8691,7 @@
         <v>4</v>
       </c>
       <c r="C302" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D302" t="s">
         <v>754</v>
@@ -8713,7 +8711,7 @@
         <v>4</v>
       </c>
       <c r="C303" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D303" t="s">
         <v>756</v>
@@ -8744,7 +8742,7 @@
         <v>4</v>
       </c>
       <c r="C305" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D305" t="s">
         <v>760</v>
@@ -8775,7 +8773,7 @@
         <v>4</v>
       </c>
       <c r="C307" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D307" t="s">
         <v>765</v>
@@ -8820,7 +8818,7 @@
         <v>4</v>
       </c>
       <c r="C310" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D310" t="s">
         <v>772</v>
@@ -8840,7 +8838,7 @@
         <v>4</v>
       </c>
       <c r="C311" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D311" t="s">
         <v>774</v>
@@ -8871,7 +8869,7 @@
         <v>4</v>
       </c>
       <c r="C313" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D313" t="s">
         <v>778</v>
@@ -8891,7 +8889,7 @@
         <v>4</v>
       </c>
       <c r="C314" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D314" t="s">
         <v>781</v>
@@ -8922,7 +8920,7 @@
         <v>4</v>
       </c>
       <c r="C316" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D316" t="s">
         <v>786</v>
@@ -8942,7 +8940,7 @@
         <v>4</v>
       </c>
       <c r="C317" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D317" t="s">
         <v>788</v>
@@ -8973,7 +8971,7 @@
         <v>4</v>
       </c>
       <c r="C319" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D319" t="s">
         <v>793</v>
@@ -9004,7 +9002,7 @@
         <v>4</v>
       </c>
       <c r="C321" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D321" t="s">
         <v>798</v>
@@ -9024,7 +9022,7 @@
         <v>4</v>
       </c>
       <c r="C322" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D322" t="s">
         <v>801</v>
@@ -9069,7 +9067,7 @@
         <v>4</v>
       </c>
       <c r="C325" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D325" t="s">
         <v>808</v>
@@ -9114,7 +9112,7 @@
         <v>4</v>
       </c>
       <c r="C328" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D328" t="s">
         <v>816</v>
@@ -9134,7 +9132,7 @@
         <v>4</v>
       </c>
       <c r="C329" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D329" t="s">
         <v>819</v>
@@ -9165,7 +9163,7 @@
         <v>4</v>
       </c>
       <c r="C331" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D331" t="s">
         <v>823</v>
@@ -9221,7 +9219,7 @@
         <v>4</v>
       </c>
       <c r="C335" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D335" t="s">
         <v>833</v>
@@ -9241,7 +9239,7 @@
         <v>4</v>
       </c>
       <c r="C336" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D336" t="s">
         <v>836</v>
@@ -9286,7 +9284,7 @@
         <v>4</v>
       </c>
       <c r="C339" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D339" t="s">
         <v>842</v>
@@ -9331,7 +9329,7 @@
         <v>4</v>
       </c>
       <c r="C342" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D342" t="s">
         <v>848</v>
@@ -9351,7 +9349,7 @@
         <v>4</v>
       </c>
       <c r="C343" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D343" t="s">
         <v>851</v>
@@ -9382,7 +9380,7 @@
         <v>4</v>
       </c>
       <c r="C345" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D345" t="s">
         <v>856</v>
@@ -9413,7 +9411,7 @@
         <v>4</v>
       </c>
       <c r="C347" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D347" t="s">
         <v>861</v>
@@ -9435,13 +9433,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8EE66F-5BF1-6F47-9F88-8D8C53839AC6}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="54.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="161.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -9488,7 +9486,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9496,10 +9494,10 @@
         <v>899</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9507,7 +9505,7 @@
         <v>900</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>905</v>
+        <v>920</v>
       </c>
     </row>
   </sheetData>
@@ -9538,26 +9536,26 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="B2" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="B3" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B4" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improve cyfun scores definition
</commit_message>
<xml_diff>
--- a/tools/ccb/ccb-cff-2023-03-01.xlsx
+++ b/tools/ccb/ccb-cff-2023-03-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/ccb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC6BB1A-58AC-184B-8FEA-C488728ACD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBF23A2-3786-1B49-833B-C2559CA6FA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2938,15 +2938,6 @@
     <t>Optimizing</t>
   </si>
   <si>
-    <t>Process unpredictable, reactive, not documented &amp; poorly controlled</t>
-  </si>
-  <si>
-    <t>Ad Hoc Processes, mostly informal, project oriented &amp; often reactive</t>
-  </si>
-  <si>
-    <t>Formal processes, organisation oriented &amp; proactive</t>
-  </si>
-  <si>
     <t>scores</t>
   </si>
   <si>
@@ -2993,19 +2984,42 @@
 https://ccb.belgium.be</t>
   </si>
   <si>
-    <t>Formal processes, organisation oriented, controlled, proactive &amp; measured</t>
-  </si>
-  <si>
-    <t>Formal processes, organisation oriented, controlled, proactive, measured &amp; continual improvement focus</t>
+    <t>No Process documentation or not formally approved by management.
+Standard process does not exist.</t>
+  </si>
+  <si>
+    <t>Formally approved Process documentation exists but not reviewed in the previous 2 years.
+Ad-hoc process exists and is done informally.</t>
+  </si>
+  <si>
+    <t>Formally approved Process documentation exists, and exceptions are documented and approved. Documented &amp; approved exceptions &lt; 5% of the time.
+Formal process exists and is implemented. Evidence available for most activities. Less than 10% process exceptions.</t>
+  </si>
+  <si>
+    <t>Formally approved Process documentation exists, and exceptions are documented and approved. Documented &amp; approved exceptions &lt; 3% of the time.
+Formal process exists and is implemented. Evidence available for all activities. Detailed metrics of the process are captured and reported.
+Minimal target for metrics has been established. Less than 5% of process exceptions.</t>
+  </si>
+  <si>
+    <t>Formally approved Process documentation exists, and exceptions are documented and approved. Documented &amp; approved exceptions &lt; 0,5% of the time.
+Formal process exists and is implemented. Evidence available for all activities. Detailed metrics of the process are captured and reported.
+Minimal target for metrics has been established and continually improving. Less than 1% of process exceptions.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3059,23 +3073,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3437,7 +3458,7 @@
         <v>874</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -3512,10 +3533,10 @@
         <v>887</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="C15" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3523,10 +3544,10 @@
         <v>887</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="C16" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
     </row>
   </sheetData>
@@ -3562,7 +3583,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>864</v>
@@ -3621,7 +3642,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -3641,7 +3662,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -3661,7 +3682,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
@@ -3681,7 +3702,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
@@ -3712,7 +3733,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
@@ -3732,7 +3753,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
@@ -3752,7 +3773,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -3772,7 +3793,7 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D13" t="s">
         <v>35</v>
@@ -3792,7 +3813,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D14" t="s">
         <v>38</v>
@@ -3823,7 +3844,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D16" t="s">
         <v>43</v>
@@ -3843,7 +3864,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D17" t="s">
         <v>46</v>
@@ -3863,7 +3884,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D18" t="s">
         <v>49</v>
@@ -3894,7 +3915,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D20" t="s">
         <v>54</v>
@@ -3914,7 +3935,7 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D21" t="s">
         <v>57</v>
@@ -3945,7 +3966,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D23" t="s">
         <v>62</v>
@@ -3976,7 +3997,7 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D25" t="s">
         <v>67</v>
@@ -3996,7 +4017,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D26" t="s">
         <v>70</v>
@@ -4041,7 +4062,7 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D29" t="s">
         <v>78</v>
@@ -4061,7 +4082,7 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D30" t="s">
         <v>81</v>
@@ -4092,7 +4113,7 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D32" t="s">
         <v>890</v>
@@ -4123,7 +4144,7 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D34" t="s">
         <v>891</v>
@@ -4154,7 +4175,7 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D36" t="s">
         <v>892</v>
@@ -4185,7 +4206,7 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D38" t="s">
         <v>97</v>
@@ -4205,7 +4226,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D39" t="s">
         <v>100</v>
@@ -4225,7 +4246,7 @@
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D40" t="s">
         <v>103</v>
@@ -4270,7 +4291,7 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D43" t="s">
         <v>111</v>
@@ -4290,7 +4311,7 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D44" t="s">
         <v>114</v>
@@ -4321,7 +4342,7 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D46" t="s">
         <v>119</v>
@@ -4341,7 +4362,7 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D47" t="s">
         <v>122</v>
@@ -4372,7 +4393,7 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D49" t="s">
         <v>127</v>
@@ -4392,7 +4413,7 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D50" t="s">
         <v>130</v>
@@ -4437,7 +4458,7 @@
         <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D53" t="s">
         <v>138</v>
@@ -4457,7 +4478,7 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D54" t="s">
         <v>141</v>
@@ -4477,7 +4498,7 @@
         <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D55" t="s">
         <v>144</v>
@@ -4508,7 +4529,7 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D57" t="s">
         <v>149</v>
@@ -4528,7 +4549,7 @@
         <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D58" t="s">
         <v>152</v>
@@ -4559,7 +4580,7 @@
         <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D60" t="s">
         <v>156</v>
@@ -4579,7 +4600,7 @@
         <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D61" t="s">
         <v>159</v>
@@ -4599,7 +4620,7 @@
         <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D62" t="s">
         <v>162</v>
@@ -4630,7 +4651,7 @@
         <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D64" t="s">
         <v>166</v>
@@ -4675,7 +4696,7 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D67" t="s">
         <v>174</v>
@@ -4706,7 +4727,7 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D69" t="s">
         <v>179</v>
@@ -4737,7 +4758,7 @@
         <v>4</v>
       </c>
       <c r="C71" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D71" t="s">
         <v>184</v>
@@ -4782,7 +4803,7 @@
         <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D74" t="s">
         <v>191</v>
@@ -4813,7 +4834,7 @@
         <v>4</v>
       </c>
       <c r="C76" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D76" t="s">
         <v>195</v>
@@ -4833,7 +4854,7 @@
         <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D77" t="s">
         <v>198</v>
@@ -4864,7 +4885,7 @@
         <v>4</v>
       </c>
       <c r="C79" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D79" t="s">
         <v>203</v>
@@ -4884,7 +4905,7 @@
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D80" t="s">
         <v>206</v>
@@ -4904,7 +4925,7 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D81" t="s">
         <v>209</v>
@@ -4935,7 +4956,7 @@
         <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D83" t="s">
         <v>213</v>
@@ -4955,7 +4976,7 @@
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D84" t="s">
         <v>216</v>
@@ -4986,7 +5007,7 @@
         <v>4</v>
       </c>
       <c r="C86" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D86" t="s">
         <v>221</v>
@@ -5006,7 +5027,7 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D87" t="s">
         <v>223</v>
@@ -5062,13 +5083,13 @@
         <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D91" t="s">
         <v>232</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>233</v>
@@ -5082,7 +5103,7 @@
         <v>4</v>
       </c>
       <c r="C92" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D92" t="s">
         <v>234</v>
@@ -5102,7 +5123,7 @@
         <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D93" t="s">
         <v>237</v>
@@ -5122,7 +5143,7 @@
         <v>4</v>
       </c>
       <c r="C94" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D94" t="s">
         <v>240</v>
@@ -5142,7 +5163,7 @@
         <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D95" t="s">
         <v>243</v>
@@ -5173,7 +5194,7 @@
         <v>4</v>
       </c>
       <c r="C97" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D97" t="s">
         <v>248</v>
@@ -5193,7 +5214,7 @@
         <v>4</v>
       </c>
       <c r="C98" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D98" t="s">
         <v>251</v>
@@ -5213,7 +5234,7 @@
         <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D99" t="s">
         <v>254</v>
@@ -5233,7 +5254,7 @@
         <v>4</v>
       </c>
       <c r="C100" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D100" t="s">
         <v>257</v>
@@ -5264,7 +5285,7 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D102" t="s">
         <v>262</v>
@@ -5284,7 +5305,7 @@
         <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D103" t="s">
         <v>265</v>
@@ -5304,7 +5325,7 @@
         <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D104" t="s">
         <v>268</v>
@@ -5324,7 +5345,7 @@
         <v>4</v>
       </c>
       <c r="C105" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D105" t="s">
         <v>271</v>
@@ -5344,7 +5365,7 @@
         <v>4</v>
       </c>
       <c r="C106" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D106" t="s">
         <v>274</v>
@@ -5375,7 +5396,7 @@
         <v>4</v>
       </c>
       <c r="C108" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D108" t="s">
         <v>279</v>
@@ -5395,7 +5416,7 @@
         <v>4</v>
       </c>
       <c r="C109" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D109" t="s">
         <v>282</v>
@@ -5415,13 +5436,13 @@
         <v>4</v>
       </c>
       <c r="C110" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D110" t="s">
         <v>285</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="G110" s="4" t="s">
         <v>286</v>
@@ -5435,13 +5456,13 @@
         <v>4</v>
       </c>
       <c r="C111" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D111" t="s">
         <v>287</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="G111" s="4" t="s">
         <v>288</v>
@@ -5455,7 +5476,7 @@
         <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D112" t="s">
         <v>289</v>
@@ -5475,7 +5496,7 @@
         <v>4</v>
       </c>
       <c r="C113" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D113" t="s">
         <v>292</v>
@@ -5495,7 +5516,7 @@
         <v>4</v>
       </c>
       <c r="C114" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D114" t="s">
         <v>295</v>
@@ -5515,7 +5536,7 @@
         <v>4</v>
       </c>
       <c r="C115" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D115" t="s">
         <v>297</v>
@@ -5535,7 +5556,7 @@
         <v>4</v>
       </c>
       <c r="C116" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D116" t="s">
         <v>300</v>
@@ -5566,7 +5587,7 @@
         <v>4</v>
       </c>
       <c r="C118" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D118" t="s">
         <v>304</v>
@@ -5586,7 +5607,7 @@
         <v>4</v>
       </c>
       <c r="C119" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D119" t="s">
         <v>307</v>
@@ -5606,7 +5627,7 @@
         <v>4</v>
       </c>
       <c r="C120" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D120" t="s">
         <v>310</v>
@@ -5626,7 +5647,7 @@
         <v>4</v>
       </c>
       <c r="C121" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D121" t="s">
         <v>313</v>
@@ -5646,7 +5667,7 @@
         <v>4</v>
       </c>
       <c r="C122" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D122" t="s">
         <v>316</v>
@@ -5666,7 +5687,7 @@
         <v>4</v>
       </c>
       <c r="C123" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D123" t="s">
         <v>318</v>
@@ -5697,7 +5718,7 @@
         <v>4</v>
       </c>
       <c r="C125" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D125" t="s">
         <v>322</v>
@@ -5717,7 +5738,7 @@
         <v>4</v>
       </c>
       <c r="C126" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D126" t="s">
         <v>324</v>
@@ -5748,7 +5769,7 @@
         <v>4</v>
       </c>
       <c r="C128" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D128" t="s">
         <v>328</v>
@@ -5793,7 +5814,7 @@
         <v>4</v>
       </c>
       <c r="C131" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D131" t="s">
         <v>336</v>
@@ -5813,7 +5834,7 @@
         <v>4</v>
       </c>
       <c r="C132" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D132" t="s">
         <v>339</v>
@@ -5833,7 +5854,7 @@
         <v>4</v>
       </c>
       <c r="C133" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D133" t="s">
         <v>342</v>
@@ -5864,7 +5885,7 @@
         <v>4</v>
       </c>
       <c r="C135" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D135" t="s">
         <v>346</v>
@@ -5895,7 +5916,7 @@
         <v>4</v>
       </c>
       <c r="C137" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D137" t="s">
         <v>350</v>
@@ -5915,7 +5936,7 @@
         <v>4</v>
       </c>
       <c r="C138" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D138" t="s">
         <v>353</v>
@@ -5935,7 +5956,7 @@
         <v>4</v>
       </c>
       <c r="C139" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D139" t="s">
         <v>356</v>
@@ -5955,7 +5976,7 @@
         <v>4</v>
       </c>
       <c r="C140" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D140" t="s">
         <v>359</v>
@@ -5986,7 +6007,7 @@
         <v>4</v>
       </c>
       <c r="C142" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D142" t="s">
         <v>363</v>
@@ -6017,7 +6038,7 @@
         <v>4</v>
       </c>
       <c r="C144" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D144" t="s">
         <v>368</v>
@@ -6062,7 +6083,7 @@
         <v>4</v>
       </c>
       <c r="C147" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D147" t="s">
         <v>375</v>
@@ -6093,7 +6114,7 @@
         <v>4</v>
       </c>
       <c r="C149" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D149" t="s">
         <v>380</v>
@@ -6124,7 +6145,7 @@
         <v>4</v>
       </c>
       <c r="C151" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D151" t="s">
         <v>385</v>
@@ -6144,7 +6165,7 @@
         <v>4</v>
       </c>
       <c r="C152" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D152" t="s">
         <v>388</v>
@@ -6164,7 +6185,7 @@
         <v>4</v>
       </c>
       <c r="C153" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D153" t="s">
         <v>391</v>
@@ -6184,7 +6205,7 @@
         <v>4</v>
       </c>
       <c r="C154" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D154" t="s">
         <v>394</v>
@@ -6215,7 +6236,7 @@
         <v>4</v>
       </c>
       <c r="C156" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D156" t="s">
         <v>399</v>
@@ -6235,7 +6256,7 @@
         <v>4</v>
       </c>
       <c r="C157" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D157" t="s">
         <v>893</v>
@@ -6255,7 +6276,7 @@
         <v>4</v>
       </c>
       <c r="C158" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D158" t="s">
         <v>403</v>
@@ -6286,7 +6307,7 @@
         <v>4</v>
       </c>
       <c r="C160" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D160" t="s">
         <v>407</v>
@@ -6317,7 +6338,7 @@
         <v>4</v>
       </c>
       <c r="C162" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D162" t="s">
         <v>412</v>
@@ -6337,7 +6358,7 @@
         <v>4</v>
       </c>
       <c r="C163" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D163" t="s">
         <v>415</v>
@@ -6357,7 +6378,7 @@
         <v>4</v>
       </c>
       <c r="C164" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D164" t="s">
         <v>417</v>
@@ -6388,7 +6409,7 @@
         <v>4</v>
       </c>
       <c r="C166" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D166" t="s">
         <v>421</v>
@@ -6419,7 +6440,7 @@
         <v>4</v>
       </c>
       <c r="C168" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D168" t="s">
         <v>426</v>
@@ -6439,7 +6460,7 @@
         <v>4</v>
       </c>
       <c r="C169" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D169" t="s">
         <v>428</v>
@@ -6462,7 +6483,7 @@
         <v>431</v>
       </c>
       <c r="F170" s="4" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -6484,7 +6505,7 @@
         <v>4</v>
       </c>
       <c r="C172" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D172" t="s">
         <v>434</v>
@@ -6504,7 +6525,7 @@
         <v>4</v>
       </c>
       <c r="C173" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D173" t="s">
         <v>437</v>
@@ -6535,7 +6556,7 @@
         <v>4</v>
       </c>
       <c r="C175" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D175" t="s">
         <v>442</v>
@@ -6555,7 +6576,7 @@
         <v>4</v>
       </c>
       <c r="C176" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D176" t="s">
         <v>445</v>
@@ -6586,7 +6607,7 @@
         <v>4</v>
       </c>
       <c r="C178" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D178" t="s">
         <v>450</v>
@@ -6606,7 +6627,7 @@
         <v>4</v>
       </c>
       <c r="C179" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D179" t="s">
         <v>452</v>
@@ -6637,7 +6658,7 @@
         <v>4</v>
       </c>
       <c r="C181" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D181" t="s">
         <v>456</v>
@@ -6657,7 +6678,7 @@
         <v>4</v>
       </c>
       <c r="C182" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D182" t="s">
         <v>459</v>
@@ -6677,7 +6698,7 @@
         <v>4</v>
       </c>
       <c r="C183" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D183" t="s">
         <v>462</v>
@@ -6697,7 +6718,7 @@
         <v>4</v>
       </c>
       <c r="C184" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D184" t="s">
         <v>465</v>
@@ -6717,7 +6738,7 @@
         <v>4</v>
       </c>
       <c r="C185" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D185" t="s">
         <v>468</v>
@@ -6748,7 +6769,7 @@
         <v>4</v>
       </c>
       <c r="C187" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D187" t="s">
         <v>473</v>
@@ -6768,7 +6789,7 @@
         <v>4</v>
       </c>
       <c r="C188" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D188" t="s">
         <v>476</v>
@@ -6799,7 +6820,7 @@
         <v>4</v>
       </c>
       <c r="C190" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D190" t="s">
         <v>480</v>
@@ -6819,7 +6840,7 @@
         <v>4</v>
       </c>
       <c r="C191" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D191" t="s">
         <v>483</v>
@@ -6850,7 +6871,7 @@
         <v>4</v>
       </c>
       <c r="C193" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D193" t="s">
         <v>488</v>
@@ -6870,7 +6891,7 @@
         <v>4</v>
       </c>
       <c r="C194" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D194" t="s">
         <v>490</v>
@@ -6890,7 +6911,7 @@
         <v>4</v>
       </c>
       <c r="C195" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D195" t="s">
         <v>493</v>
@@ -6921,7 +6942,7 @@
         <v>4</v>
       </c>
       <c r="C197" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D197" t="s">
         <v>497</v>
@@ -6941,7 +6962,7 @@
         <v>4</v>
       </c>
       <c r="C198" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D198" t="s">
         <v>499</v>
@@ -6961,7 +6982,7 @@
         <v>4</v>
       </c>
       <c r="C199" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D199" t="s">
         <v>501</v>
@@ -6992,7 +7013,7 @@
         <v>4</v>
       </c>
       <c r="C201" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D201" t="s">
         <v>505</v>
@@ -7012,7 +7033,7 @@
         <v>4</v>
       </c>
       <c r="C202" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D202" t="s">
         <v>508</v>
@@ -7043,7 +7064,7 @@
         <v>4</v>
       </c>
       <c r="C204" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D204" t="s">
         <v>513</v>
@@ -7063,7 +7084,7 @@
         <v>4</v>
       </c>
       <c r="C205" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D205" t="s">
         <v>516</v>
@@ -7094,7 +7115,7 @@
         <v>4</v>
       </c>
       <c r="C207" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D207" t="s">
         <v>521</v>
@@ -7139,7 +7160,7 @@
         <v>4</v>
       </c>
       <c r="C210" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D210" t="s">
         <v>529</v>
@@ -7159,7 +7180,7 @@
         <v>4</v>
       </c>
       <c r="C211" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D211" t="s">
         <v>532</v>
@@ -7179,7 +7200,7 @@
         <v>4</v>
       </c>
       <c r="C212" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D212" t="s">
         <v>535</v>
@@ -7199,7 +7220,7 @@
         <v>4</v>
       </c>
       <c r="C213" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D213" t="s">
         <v>538</v>
@@ -7219,7 +7240,7 @@
         <v>4</v>
       </c>
       <c r="C214" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D214" t="s">
         <v>541</v>
@@ -7239,7 +7260,7 @@
         <v>4</v>
       </c>
       <c r="C215" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D215" t="s">
         <v>544</v>
@@ -7259,7 +7280,7 @@
         <v>4</v>
       </c>
       <c r="C216" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D216" t="s">
         <v>546</v>
@@ -7290,7 +7311,7 @@
         <v>4</v>
       </c>
       <c r="C218" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D218" t="s">
         <v>550</v>
@@ -7310,7 +7331,7 @@
         <v>4</v>
       </c>
       <c r="C219" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D219" t="s">
         <v>552</v>
@@ -7330,7 +7351,7 @@
         <v>4</v>
       </c>
       <c r="C220" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D220" t="s">
         <v>554</v>
@@ -7375,7 +7396,7 @@
         <v>4</v>
       </c>
       <c r="C223" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D223" t="s">
         <v>561</v>
@@ -7395,7 +7416,7 @@
         <v>4</v>
       </c>
       <c r="C224" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D224" t="s">
         <v>564</v>
@@ -7415,7 +7436,7 @@
         <v>4</v>
       </c>
       <c r="C225" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D225" t="s">
         <v>567</v>
@@ -7435,7 +7456,7 @@
         <v>4</v>
       </c>
       <c r="C226" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D226" t="s">
         <v>570</v>
@@ -7466,7 +7487,7 @@
         <v>4</v>
       </c>
       <c r="C228" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D228" t="s">
         <v>574</v>
@@ -7486,7 +7507,7 @@
         <v>4</v>
       </c>
       <c r="C229" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D229" t="s">
         <v>576</v>
@@ -7506,7 +7527,7 @@
         <v>4</v>
       </c>
       <c r="C230" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D230" t="s">
         <v>578</v>
@@ -7537,7 +7558,7 @@
         <v>4</v>
       </c>
       <c r="C232" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D232" t="s">
         <v>583</v>
@@ -7557,7 +7578,7 @@
         <v>4</v>
       </c>
       <c r="C233" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D233" t="s">
         <v>586</v>
@@ -7577,7 +7598,7 @@
         <v>4</v>
       </c>
       <c r="C234" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D234" t="s">
         <v>588</v>
@@ -7608,7 +7629,7 @@
         <v>4</v>
       </c>
       <c r="C236" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D236" t="s">
         <v>592</v>
@@ -7628,7 +7649,7 @@
         <v>4</v>
       </c>
       <c r="C237" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D237" t="s">
         <v>595</v>
@@ -7648,7 +7669,7 @@
         <v>4</v>
       </c>
       <c r="C238" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D238" t="s">
         <v>598</v>
@@ -7704,7 +7725,7 @@
         <v>4</v>
       </c>
       <c r="C242" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D242" t="s">
         <v>607</v>
@@ -7735,7 +7756,7 @@
         <v>4</v>
       </c>
       <c r="C244" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D244" t="s">
         <v>612</v>
@@ -7755,7 +7776,7 @@
         <v>4</v>
       </c>
       <c r="C245" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D245" t="s">
         <v>614</v>
@@ -7786,7 +7807,7 @@
         <v>4</v>
       </c>
       <c r="C247" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D247" t="s">
         <v>619</v>
@@ -7806,7 +7827,7 @@
         <v>4</v>
       </c>
       <c r="C248" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D248" t="s">
         <v>622</v>
@@ -7826,7 +7847,7 @@
         <v>4</v>
       </c>
       <c r="C249" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D249" t="s">
         <v>624</v>
@@ -7857,7 +7878,7 @@
         <v>4</v>
       </c>
       <c r="C251" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D251" t="s">
         <v>628</v>
@@ -7888,7 +7909,7 @@
         <v>4</v>
       </c>
       <c r="C253" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D253" t="s">
         <v>632</v>
@@ -7908,7 +7929,7 @@
         <v>4</v>
       </c>
       <c r="C254" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D254" t="s">
         <v>634</v>
@@ -7953,7 +7974,7 @@
         <v>4</v>
       </c>
       <c r="C257" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D257" t="s">
         <v>641</v>
@@ -7973,7 +7994,7 @@
         <v>4</v>
       </c>
       <c r="C258" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D258" t="s">
         <v>644</v>
@@ -7993,7 +8014,7 @@
         <v>4</v>
       </c>
       <c r="C259" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D259" t="s">
         <v>647</v>
@@ -8024,7 +8045,7 @@
         <v>4</v>
       </c>
       <c r="C261" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D261" t="s">
         <v>652</v>
@@ -8044,7 +8065,7 @@
         <v>4</v>
       </c>
       <c r="C262" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D262" t="s">
         <v>654</v>
@@ -8075,7 +8096,7 @@
         <v>4</v>
       </c>
       <c r="C264" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D264" t="s">
         <v>659</v>
@@ -8095,7 +8116,7 @@
         <v>4</v>
       </c>
       <c r="C265" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D265" t="s">
         <v>662</v>
@@ -8115,7 +8136,7 @@
         <v>4</v>
       </c>
       <c r="C266" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D266" t="s">
         <v>665</v>
@@ -8146,7 +8167,7 @@
         <v>4</v>
       </c>
       <c r="C268" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D268" t="s">
         <v>670</v>
@@ -8166,7 +8187,7 @@
         <v>4</v>
       </c>
       <c r="C269" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D269" t="s">
         <v>673</v>
@@ -8197,7 +8218,7 @@
         <v>4</v>
       </c>
       <c r="C271" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D271" t="s">
         <v>677</v>
@@ -8228,7 +8249,7 @@
         <v>4</v>
       </c>
       <c r="C273" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D273" t="s">
         <v>682</v>
@@ -8248,7 +8269,7 @@
         <v>4</v>
       </c>
       <c r="C274" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D274" t="s">
         <v>685</v>
@@ -8279,7 +8300,7 @@
         <v>4</v>
       </c>
       <c r="C276" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D276" t="s">
         <v>689</v>
@@ -8299,7 +8320,7 @@
         <v>4</v>
       </c>
       <c r="C277" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D277" t="s">
         <v>692</v>
@@ -8330,7 +8351,7 @@
         <v>4</v>
       </c>
       <c r="C279" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D279" t="s">
         <v>696</v>
@@ -8350,7 +8371,7 @@
         <v>4</v>
       </c>
       <c r="C280" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D280" t="s">
         <v>699</v>
@@ -8395,7 +8416,7 @@
         <v>4</v>
       </c>
       <c r="C283" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D283" t="s">
         <v>706</v>
@@ -8426,7 +8447,7 @@
         <v>4</v>
       </c>
       <c r="C285" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D285" t="s">
         <v>710</v>
@@ -8457,7 +8478,7 @@
         <v>4</v>
       </c>
       <c r="C287" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D287" t="s">
         <v>715</v>
@@ -8488,7 +8509,7 @@
         <v>4</v>
       </c>
       <c r="C289" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D289" t="s">
         <v>720</v>
@@ -8508,7 +8529,7 @@
         <v>4</v>
       </c>
       <c r="C290" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D290" t="s">
         <v>723</v>
@@ -8564,7 +8585,7 @@
         <v>4</v>
       </c>
       <c r="C294" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D294" t="s">
         <v>733</v>
@@ -8609,7 +8630,7 @@
         <v>4</v>
       </c>
       <c r="C297" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D297" t="s">
         <v>741</v>
@@ -8640,7 +8661,7 @@
         <v>4</v>
       </c>
       <c r="C299" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D299" t="s">
         <v>746</v>
@@ -8660,7 +8681,7 @@
         <v>4</v>
       </c>
       <c r="C300" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D300" t="s">
         <v>749</v>
@@ -8691,7 +8712,7 @@
         <v>4</v>
       </c>
       <c r="C302" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D302" t="s">
         <v>754</v>
@@ -8711,7 +8732,7 @@
         <v>4</v>
       </c>
       <c r="C303" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D303" t="s">
         <v>756</v>
@@ -8742,7 +8763,7 @@
         <v>4</v>
       </c>
       <c r="C305" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D305" t="s">
         <v>760</v>
@@ -8773,7 +8794,7 @@
         <v>4</v>
       </c>
       <c r="C307" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D307" t="s">
         <v>765</v>
@@ -8818,7 +8839,7 @@
         <v>4</v>
       </c>
       <c r="C310" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D310" t="s">
         <v>772</v>
@@ -8838,7 +8859,7 @@
         <v>4</v>
       </c>
       <c r="C311" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D311" t="s">
         <v>774</v>
@@ -8869,7 +8890,7 @@
         <v>4</v>
       </c>
       <c r="C313" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D313" t="s">
         <v>778</v>
@@ -8889,7 +8910,7 @@
         <v>4</v>
       </c>
       <c r="C314" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D314" t="s">
         <v>781</v>
@@ -8920,7 +8941,7 @@
         <v>4</v>
       </c>
       <c r="C316" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D316" t="s">
         <v>786</v>
@@ -8940,7 +8961,7 @@
         <v>4</v>
       </c>
       <c r="C317" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D317" t="s">
         <v>788</v>
@@ -8971,7 +8992,7 @@
         <v>4</v>
       </c>
       <c r="C319" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D319" t="s">
         <v>793</v>
@@ -9002,7 +9023,7 @@
         <v>4</v>
       </c>
       <c r="C321" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D321" t="s">
         <v>798</v>
@@ -9022,7 +9043,7 @@
         <v>4</v>
       </c>
       <c r="C322" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D322" t="s">
         <v>801</v>
@@ -9067,7 +9088,7 @@
         <v>4</v>
       </c>
       <c r="C325" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D325" t="s">
         <v>808</v>
@@ -9112,7 +9133,7 @@
         <v>4</v>
       </c>
       <c r="C328" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D328" t="s">
         <v>816</v>
@@ -9132,7 +9153,7 @@
         <v>4</v>
       </c>
       <c r="C329" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D329" t="s">
         <v>819</v>
@@ -9163,7 +9184,7 @@
         <v>4</v>
       </c>
       <c r="C331" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D331" t="s">
         <v>823</v>
@@ -9219,7 +9240,7 @@
         <v>4</v>
       </c>
       <c r="C335" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="D335" t="s">
         <v>833</v>
@@ -9239,7 +9260,7 @@
         <v>4</v>
       </c>
       <c r="C336" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D336" t="s">
         <v>836</v>
@@ -9284,7 +9305,7 @@
         <v>4</v>
       </c>
       <c r="C339" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D339" t="s">
         <v>842</v>
@@ -9329,7 +9350,7 @@
         <v>4</v>
       </c>
       <c r="C342" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D342" t="s">
         <v>848</v>
@@ -9349,7 +9370,7 @@
         <v>4</v>
       </c>
       <c r="C343" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D343" t="s">
         <v>851</v>
@@ -9380,7 +9401,7 @@
         <v>4</v>
       </c>
       <c r="C345" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D345" t="s">
         <v>856</v>
@@ -9411,7 +9432,7 @@
         <v>4</v>
       </c>
       <c r="C347" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="D347" t="s">
         <v>861</v>
@@ -9433,78 +9454,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8EE66F-5BF1-6F47-9F88-8D8C53839AC6}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="161.1640625" customWidth="1"/>
+    <col min="1" max="2" width="10.83203125" style="7"/>
+    <col min="3" max="3" width="161.1640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>895</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>896</v>
       </c>
-      <c r="C2" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="C2" s="8" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>897</v>
       </c>
-      <c r="C3" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C3" s="9" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>898</v>
       </c>
-      <c r="C4" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C4" s="9" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>899</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="9" t="s">
         <v>919</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>900</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="9" t="s">
         <v>920</v>
       </c>
     </row>
@@ -9536,26 +9560,26 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>903</v>
+      </c>
+      <c r="B2" t="s">
         <v>906</v>
-      </c>
-      <c r="B2" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>904</v>
+      </c>
+      <c r="B3" t="s">
         <v>907</v>
-      </c>
-      <c r="B3" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>905</v>
+      </c>
+      <c r="B4" t="s">
         <v>908</v>
-      </c>
-      <c r="B4" t="s">
-        <v>911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix errors in score definitions
- add min_score and max_score to CCB et NIST CSF v2
- fix NIST CSF score 1
- update versions
</commit_message>
<xml_diff>
--- a/tools/ccb/ccb-cff-2023-03-01.xlsx
+++ b/tools/ccb/ccb-cff-2023-03-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/ccb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBF23A2-3786-1B49-833B-C2559CA6FA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BAEEAA-87F3-934D-8892-F19C4B0887FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="923">
   <si>
     <t>assessable</t>
   </si>
@@ -3004,6 +3004,12 @@
     <t>Formally approved Process documentation exists, and exceptions are documented and approved. Documented &amp; approved exceptions &lt; 0,5% of the time.
 Formal process exists and is implemented. Evidence available for all activities. Detailed metrics of the process are captured and reported.
 Minimal target for metrics has been established and continually improving. Less than 1% of process exceptions.</t>
+  </si>
+  <si>
+    <t>framework_min_score</t>
+  </si>
+  <si>
+    <t>framework_max_score</t>
   </si>
 </sst>
 </file>
@@ -3073,7 +3079,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -3091,12 +3097,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3400,10 +3402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B1651-6DC7-1E43-A5B6-8EF15B32842F}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScale="231" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="231" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3426,7 +3428,7 @@
         <v>867</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3519,24 +3521,18 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>887</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>888</v>
-      </c>
-      <c r="C14" t="s">
-        <v>889</v>
+        <v>921</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>887</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>901</v>
-      </c>
-      <c r="C15" t="s">
-        <v>901</v>
+        <v>922</v>
+      </c>
+      <c r="B15" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -3544,9 +3540,31 @@
         <v>887</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="C16" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>887</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="C17" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>887</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>902</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>902</v>
       </c>
     </row>
@@ -9454,81 +9472,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8EE66F-5BF1-6F47-9F88-8D8C53839AC6}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="7"/>
-    <col min="3" max="3" width="161.1640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="30.1640625" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="7"/>
+    <col min="3" max="3" width="161.1640625" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" t="s">
         <v>895</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" t="s">
         <v>894</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>896</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>916</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" t="s">
         <v>897</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>917</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>898</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="4" t="s">
         <v>918</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>899</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="4" t="s">
         <v>919</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" t="s">
         <v>900</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>920</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Use plural for IG
key measures
</commit_message>
<xml_diff>
--- a/tools/ccb/ccb-cff-2023-03-01.xlsx
+++ b/tools/ccb/ccb-cff-2023-03-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/ccb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0124940-EB5E-564C-8F13-91C6972E6548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84376F9D-3411-264B-913C-AF0DA89BC8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="22700" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22700" windowHeight="20520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -2938,19 +2938,10 @@
     <t>BK</t>
   </si>
   <si>
-    <t>basic - key measure</t>
-  </si>
-  <si>
     <t>IK</t>
   </si>
   <si>
     <t>EK</t>
-  </si>
-  <si>
-    <t>important - key measure</t>
-  </si>
-  <si>
-    <t>essential - key measure</t>
   </si>
   <si>
     <t>I,E,IK,EK</t>
@@ -3053,6 +3044,15 @@
   </si>
   <si>
     <t>[KEY MEASURE for ESSENTIAL] The organization shall perform a documented risk assessment on organization's critical system transactions and authenticate users, devices, and other assets (e.g., single-factor, multi-factor) commensurate with the risk of the transaction (e.g., individuals’ security and privacy risks and other organizational risks).</t>
+  </si>
+  <si>
+    <t>basic - key measures</t>
+  </si>
+  <si>
+    <t>important - key measures</t>
+  </si>
+  <si>
+    <t>essential - key measures</t>
   </si>
 </sst>
 </file>
@@ -3454,7 +3454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B1651-6DC7-1E43-A5B6-8EF15B32842F}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="231" workbookViewId="0">
+    <sheetView zoomScale="231" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -4065,13 +4065,13 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="D25" t="s">
         <v>67</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>68</v>
@@ -4973,13 +4973,13 @@
         <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="D80" t="s">
         <v>205</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>206</v>
@@ -4993,13 +4993,13 @@
         <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="D81" t="s">
         <v>207</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>34</v>
@@ -5151,13 +5151,13 @@
         <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D91" t="s">
         <v>229</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>230</v>
@@ -5373,13 +5373,13 @@
         <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D103" t="s">
         <v>262</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="G103" s="4" t="s">
         <v>263</v>
@@ -5393,13 +5393,13 @@
         <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="D104" t="s">
         <v>264</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="G104" s="4" t="s">
         <v>265</v>
@@ -5464,13 +5464,13 @@
         <v>4</v>
       </c>
       <c r="C108" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D108" t="s">
         <v>274</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="G108" s="4" t="s">
         <v>275</v>
@@ -5484,13 +5484,13 @@
         <v>4</v>
       </c>
       <c r="C109" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D109" t="s">
         <v>276</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="G109" s="4" t="s">
         <v>277</v>
@@ -5504,13 +5504,13 @@
         <v>4</v>
       </c>
       <c r="C110" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D110" t="s">
         <v>278</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="G110" s="4" t="s">
         <v>279</v>
@@ -5524,13 +5524,13 @@
         <v>4</v>
       </c>
       <c r="C111" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D111" t="s">
         <v>280</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
       <c r="G111" s="4" t="s">
         <v>281</v>
@@ -5655,13 +5655,13 @@
         <v>4</v>
       </c>
       <c r="C118" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D118" t="s">
         <v>297</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="G118" s="4" t="s">
         <v>298</v>
@@ -5675,13 +5675,13 @@
         <v>4</v>
       </c>
       <c r="C119" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D119" t="s">
         <v>299</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="G119" s="4" t="s">
         <v>300</v>
@@ -5695,13 +5695,13 @@
         <v>4</v>
       </c>
       <c r="C120" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="D120" t="s">
         <v>301</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
       <c r="G120" s="4" t="s">
         <v>302</v>
@@ -5715,13 +5715,13 @@
         <v>4</v>
       </c>
       <c r="C121" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="D121" t="s">
         <v>303</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>304</v>
@@ -5837,13 +5837,13 @@
         <v>4</v>
       </c>
       <c r="C128" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="D128" s="8" t="s">
         <v>317</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="G128" s="4" t="s">
         <v>318</v>
@@ -6375,13 +6375,13 @@
         <v>4</v>
       </c>
       <c r="C160" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="D160" t="s">
         <v>395</v>
       </c>
       <c r="F160" s="4" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="G160" s="4" t="s">
         <v>396</v>
@@ -6573,13 +6573,13 @@
         <v>4</v>
       </c>
       <c r="C172" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="D172" t="s">
         <v>421</v>
       </c>
       <c r="F172" s="4" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="G172" s="4" t="s">
         <v>422</v>
@@ -6726,13 +6726,13 @@
         <v>4</v>
       </c>
       <c r="C181" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D181" t="s">
         <v>442</v>
       </c>
       <c r="F181" s="4" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="G181" s="4" t="s">
         <v>443</v>
@@ -7228,13 +7228,13 @@
         <v>4</v>
       </c>
       <c r="C210" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D210" t="s">
         <v>514</v>
       </c>
       <c r="F210" s="4" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="G210" s="4" t="s">
         <v>515</v>
@@ -7308,13 +7308,13 @@
         <v>4</v>
       </c>
       <c r="C214" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="D214" t="s">
         <v>525</v>
       </c>
       <c r="F214" s="4" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="G214" s="4" t="s">
         <v>526</v>
@@ -7328,13 +7328,13 @@
         <v>4</v>
       </c>
       <c r="C215" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="D215" t="s">
         <v>527</v>
       </c>
       <c r="F215" s="4" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="G215" s="4" t="s">
         <v>34</v>
@@ -7348,13 +7348,13 @@
         <v>4</v>
       </c>
       <c r="C216" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="D216" t="s">
         <v>528</v>
       </c>
       <c r="F216" s="4" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="G216" s="4" t="s">
         <v>34</v>
@@ -7464,13 +7464,13 @@
         <v>4</v>
       </c>
       <c r="C223" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D223" t="s">
         <v>542</v>
       </c>
       <c r="F223" s="4" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="G223" s="4" t="s">
         <v>543</v>
@@ -7595,13 +7595,13 @@
         <v>4</v>
       </c>
       <c r="C230" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="D230" t="s">
         <v>558</v>
       </c>
       <c r="F230" s="4" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="G230" s="4" t="s">
         <v>559</v>
@@ -7793,13 +7793,13 @@
         <v>4</v>
       </c>
       <c r="C242" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="D242" t="s">
         <v>586</v>
       </c>
       <c r="F242" s="4" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="G242" s="4" t="s">
         <v>587</v>
@@ -7875,13 +7875,13 @@
         <v>4</v>
       </c>
       <c r="C247" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D247" t="s">
         <v>597</v>
       </c>
       <c r="F247" s="4" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="G247" s="4" t="s">
         <v>598</v>
@@ -8062,13 +8062,13 @@
         <v>4</v>
       </c>
       <c r="C258" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="D258" t="s">
         <v>621</v>
       </c>
       <c r="F258" s="4" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="G258" s="4" t="s">
         <v>622</v>
@@ -8235,13 +8235,13 @@
         <v>4</v>
       </c>
       <c r="C268" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D268" t="s">
         <v>646</v>
       </c>
       <c r="F268" s="4" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
       <c r="G268" s="4" t="s">
         <v>647</v>
@@ -9091,13 +9091,13 @@
         <v>4</v>
       </c>
       <c r="C321" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="D321" t="s">
         <v>773</v>
       </c>
       <c r="F321" s="4" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="G321" s="4" t="s">
         <v>774</v>
@@ -9607,8 +9607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793A9884-A8FA-0245-8718-D92EEEA60D41}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9656,23 +9656,23 @@
         <v>894</v>
       </c>
       <c r="B5" t="s">
-        <v>895</v>
+        <v>930</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B6" t="s">
-        <v>898</v>
+        <v>931</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B7" t="s">
-        <v>899</v>
+        <v>932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add missing carriage return
</commit_message>
<xml_diff>
--- a/tools/ccb/ccb-cff-2023-03-01.xlsx
+++ b/tools/ccb/ccb-cff-2023-03-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/ccb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5E0F8C-1740-D44F-983C-313BFD797315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37BFA25-BB15-A84B-9B1B-B8ABB46FA6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="2" r:id="rId1"/>
@@ -4821,33 +4821,8 @@
 Les exceptions sont documentées et approuvées dans moins de 5 % des cas.</t>
   </si>
   <si>
-    <t>Un processus formel existe et est mis en œuvre. Des preuves sont disponibles pour la plupart des activités. 
-Moins de 10 % d’exceptions au processus.</t>
-  </si>
-  <si>
-    <t>Formal process exists and is implemented. Evidence available for all activities. Detailed metrics of the process are captured and reported.
-Minimal target for metrics has been established.
-Less than 5% of process exceptions.</t>
-  </si>
-  <si>
-    <t>Formal process exists and is implemented. Evidence available for most activities.
-Less than 10% process exceptions.</t>
-  </si>
-  <si>
-    <t>Formal process exists and is implemented. Evidence available for all activities. Detailed metrics of the process are captured and reported.
-Minimal target for metrics has been established and continually improving.
-Less than 1% of process exceptions.</t>
-  </si>
-  <si>
     <t>Il existe une documentation formellement approuvée sur les processus et les exceptions sont documentées et approuvées.
 Exceptions documentées et approuvées &lt; 3 % du temps.</t>
-  </si>
-  <si>
-    <t>Un processus formel existe et est mis en œuvre. Des preuves sont disponibles pour toutes les activités. Des mesures détaillées du processus sont saisies et communiquées. Un objectif minimum est fixé pour les indicateurs.
-Moins de 5 % des exceptions au processus.</t>
-  </si>
-  <si>
-    <t>Un processus formel existe et est mis en œuvre. Des preuves sont disponibles pour toutes les activités. Des mesures détaillées du processus sont saisies et communiquées. Des objectifs minimaux sont fixés pour les indicateurs et sont améliorés en permanence. Moins de 1 % des exceptions au processus.</t>
   </si>
   <si>
     <t>Il existe une documentation formellement approuvée sur les processus et les exceptions sont documentées et approuvées.
@@ -4902,6 +4877,44 @@
     <t>Centre For Cybersecurity Belgium - CyberFondamentaux
 With content from CyFun Self-Assessment tool V2024-11-05
 https://ccb.belgium.be</t>
+  </si>
+  <si>
+    <t>Un processus formel existe et est mis en œuvre.
+Des preuves sont disponibles pour la plupart des activités. 
+Moins de 10 % d’exceptions au processus.</t>
+  </si>
+  <si>
+    <t>Un processus formel existe et est mis en œuvre.
+Des preuves sont disponibles pour toutes les activités.
+Des mesures détaillées du processus sont saisies et communiquées.
+Un objectif minimum est fixé pour les indicateurs.
+Moins de 5 % des exceptions au processus.</t>
+  </si>
+  <si>
+    <t>Un processus formel existe et est mis en œuvre.
+Des preuves sont disponibles pour toutes les activités.
+Des mesures détaillées du processus sont saisies et communiquées.
+Des objectifs minimaux sont fixés pour les indicateurs et sont améliorés en permanence.
+Moins de 1 % des exceptions au processus.</t>
+  </si>
+  <si>
+    <t>Formal process exists and is implemented.
+Evidence available for all activities.
+Detailed metrics of the process are captured and reported.
+Minimal target for metrics has been established.
+Less than 5% of process exceptions.</t>
+  </si>
+  <si>
+    <t>Formal process exists and is implemented.
+Evidence available for most activities.
+Less than 10% process exceptions.</t>
+  </si>
+  <si>
+    <t>Formal process exists and is implemented.
+Evidence available for all activities.
+Detailed metrics of the process are captured and reported.
+Minimal target for metrics has been established and continually improving.
+Less than 1% of process exceptions.</t>
   </si>
 </sst>
 </file>
@@ -5356,7 +5369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699B1651-6DC7-1E43-A5B6-8EF15B32842F}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="231" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="231" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -5385,7 +5398,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1473</v>
+        <v>1467</v>
       </c>
       <c r="B3" s="24">
         <v>45676</v>
@@ -5412,7 +5425,7 @@
         <v>845</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1472</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="48" x14ac:dyDescent="0.2">
@@ -5468,7 +5481,7 @@
         <v>857</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1472</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -5530,34 +5543,34 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1476</v>
+        <v>1470</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1480</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>1477</v>
+        <v>1471</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>1482</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1478</v>
+        <v>1472</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>1480</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>1479</v>
+        <v>1473</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1481</v>
+        <v>1475</v>
       </c>
     </row>
   </sheetData>
@@ -13976,14 +13989,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8EE66F-5BF1-6F47-9F88-8D8C53839AC6}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="3"/>
-    <col min="3" max="3" width="60.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="73.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="53.6640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="3"/>
     <col min="6" max="6" width="46.1640625" style="3" customWidth="1"/>
@@ -14002,7 +14015,7 @@
         <v>866</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>1474</v>
+        <v>1468</v>
       </c>
       <c r="E1" s="23" t="s">
         <v>1397</v>
@@ -14011,7 +14024,7 @@
         <v>1398</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>1475</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -14068,7 +14081,7 @@
         <v>870</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1461</v>
+        <v>1481</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>1447</v>
@@ -14077,7 +14090,7 @@
         <v>1451</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>1459</v>
+        <v>1477</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>1458</v>
@@ -14091,7 +14104,7 @@
         <v>871</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>1460</v>
+        <v>1480</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>1448</v>
@@ -14100,13 +14113,13 @@
         <v>1452</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>1464</v>
+        <v>1478</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>1463</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -14114,7 +14127,7 @@
         <v>872</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1462</v>
+        <v>1482</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>1449</v>
@@ -14123,10 +14136,10 @@
         <v>1453</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>1465</v>
+        <v>1479</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>1466</v>
+        <v>1460</v>
       </c>
     </row>
   </sheetData>
@@ -14174,7 +14187,7 @@
         <v>878</v>
       </c>
       <c r="D2" t="s">
-        <v>1467</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -14196,7 +14209,7 @@
         <v>880</v>
       </c>
       <c r="D4" t="s">
-        <v>1468</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -14207,7 +14220,7 @@
         <v>922</v>
       </c>
       <c r="D5" t="s">
-        <v>1469</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -14218,7 +14231,7 @@
         <v>923</v>
       </c>
       <c r="D6" t="s">
-        <v>1470</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -14229,7 +14242,7 @@
         <v>924</v>
       </c>
       <c r="D7" t="s">
-        <v>1471</v>
+        <v>1465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>